<commit_message>
prefs: add new merge (not used)
</commit_message>
<xml_diff>
--- a/_utils.xlsx
+++ b/_utils.xlsx
@@ -485,7 +485,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="4">
-        <v>45630</v>
+        <v>45633</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fix deprecated import Callable
</commit_message>
<xml_diff>
--- a/_utils.xlsx
+++ b/_utils.xlsx
@@ -488,7 +488,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="4">
-        <v>45634</v>
+        <v>45636</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
automatic copy to all projects
</commit_message>
<xml_diff>
--- a/_utils.xlsx
+++ b/_utils.xlsx
@@ -488,7 +488,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="4">
-        <v>45637</v>
+        <v>45642</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>

</xml_diff>